<commit_message>
created custome xml to xls file
</commit_message>
<xml_diff>
--- a/nirmitee_project/static/output.xlsx
+++ b/nirmitee_project/static/output.xlsx
@@ -436,22 +436,22 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ENVELOPE.HEADER.TALLYREQUEST</t>
+          <t>ENVELOPE_HEADER_TALLYREQUEST</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ENVELOPE.BODY.IMPORTDATA.REQUESTDESC.REPORTNAME</t>
+          <t>ENVELOPE_BODY_IMPORTDATA_REQUESTDESC_REPORTNAME</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ENVELOPE.BODY.IMPORTDATA.REQUESTDESC.STATICVARIABLES.SVCURRENTCOMPANY</t>
+          <t>ENVELOPE_BODY_IMPORTDATA_REQUESTDESC_STATICVARIABLES_SVCURRENTCOMPANY</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ENVELOPE.BODY.IMPORTDATA.REQUESTDATA.TALLYMESSAGE</t>
+          <t>ENVELOPE_BODY_IMPORTDATA_REQUESTDATA_TALLYMESSAGE</t>
         </is>
       </c>
     </row>

</xml_diff>